<commit_message>
Remove Input CSV from hard coded, changed Input CSV location
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -52,6 +52,30 @@
     <t xml:space="preserve">ID</t>
   </si>
   <si>
+    <t xml:space="preserve">InputPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data\Input\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TempPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data\Temp\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OutputPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data\Output\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InputFile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InputControl.csv</t>
+  </si>
+  <si>
     <t xml:space="preserve">Asset</t>
   </si>
   <si>
@@ -66,7 +90,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -96,6 +120,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,7 +170,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -154,6 +184,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,7 +208,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -184,7 +218,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.14"/>
@@ -1238,17 +1272,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="73.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.14"/>
@@ -1266,6 +1300,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1278,7 +1344,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1288,7 +1354,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="118.57"/>
@@ -1300,7 +1366,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2260,7 +2326,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2270,7 +2336,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="65.42"/>
   </cols>
@@ -2280,10 +2346,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>

</xml_diff>